<commit_message>
adds roles for add'l personnel in metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/yuba_adult_metadata.xlsx
+++ b/data-raw/metadata/yuba_adult_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/SRJPE/EDI/jpe-yuba-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BC59F8-18C6-4340-9EE7-DE7458435698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAFAD19-02F9-8B45-81E2-F04552100403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11220" yWindow="-21140" windowWidth="30240" windowHeight="17460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11220" yWindow="-21140" windowWidth="30240" windowHeight="17460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="80">
   <si>
     <t xml:space="preserve">name </t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>Monitoring adult Chinook salmon upstream passage on Yuba River</t>
+  </si>
+  <si>
+    <t>associate</t>
   </si>
 </sst>
 </file>
@@ -16785,8 +16788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16866,6 +16869,9 @@
       <c r="C4" s="20" t="s">
         <v>56</v>
       </c>
+      <c r="D4" s="17" t="s">
+        <v>79</v>
+      </c>
       <c r="E4" s="22" t="s">
         <v>53</v>
       </c>
@@ -16880,6 +16886,9 @@
       </c>
       <c r="C5" s="21" t="s">
         <v>60</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>79</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>53</v>
@@ -50144,7 +50153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updates package and validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/yuba_adult_metadata.xlsx
+++ b/data-raw/metadata/yuba_adult_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/SRJPE/EDI/jpe-yuba-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAFAD19-02F9-8B45-81E2-F04552100403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2BDF25-A291-7F41-AB48-3C5ED66848F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11220" yWindow="-21140" windowWidth="30240" windowHeight="17460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="coverage" sheetId="9" r:id="rId9"/>
     <sheet name="taxonomic_coverage" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterate="1"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mg0c4zz0CWAbM80r7xNYKHxokTpNA=="/>
@@ -272,9 +272,6 @@
     <t>annually</t>
   </si>
   <si>
-    <t>Jaso</t>
-  </si>
-  <si>
     <t>Brian</t>
   </si>
   <si>
@@ -306,6 +303,9 @@
   </si>
   <si>
     <t>associate</t>
+  </si>
+  <si>
+    <t>Jason</t>
   </si>
 </sst>
 </file>
@@ -717,7 +717,7 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -16789,7 +16789,7 @@
   <dimension ref="A1:F999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16825,37 +16825,37 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>70</v>
-      </c>
       <c r="C2" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>52</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="C3" s="17" t="s">
         <v>72</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>73</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>51</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F3" s="18"/>
     </row>
@@ -16870,7 +16870,7 @@
         <v>56</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>53</v>
@@ -16879,7 +16879,7 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>59</v>
@@ -16888,7 +16888,7 @@
         <v>60</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>53</v>
@@ -19916,10 +19916,10 @@
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -50192,7 +50192,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="16">
         <v>-121.51359600000001</v>

</xml_diff>

<commit_message>
fixes typo in instantenous metadata, fixes coverage in adult metadata, rewrites and validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/yuba_adult_metadata.xlsx
+++ b/data-raw/metadata/yuba_adult_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/SRJPE/EDI/jpe-yuba-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2BDF25-A291-7F41-AB48-3C5ED66848F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B4CE3F-6477-6E46-8B5F-5A6DCFA2E88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -16788,7 +16788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -50153,7 +50153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -50210,7 +50210,7 @@
         <v>38047</v>
       </c>
       <c r="G2" s="12">
-        <v>45288</v>
+        <v>44985</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>

</xml_diff>